<commit_message>
Remove assignees from Non_ISIS testing
Remove people from assignees list that no longer work on the Mantid project
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template_Non_ISIS.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template_Non_ISIS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39876" yWindow="4944" windowWidth="19476" windowHeight="23496"/>
+    <workbookView xWindow="39876" yWindow="4944" windowWidth="19476" windowHeight="23496" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Title</t>
   </si>
@@ -85,12 +85,6 @@
   </si>
   <si>
     <t>Jose Borreguero</t>
-  </si>
-  <si>
-    <t>martyngigg</t>
-  </si>
-  <si>
-    <t>Martyn Gigg</t>
   </si>
   <si>
     <t>mdoucet</t>
@@ -139,12 +133,6 @@
     <t>size</t>
   </si>
   <si>
-    <t>Pasarus</t>
-  </si>
-  <si>
-    <t>Sam Jones</t>
-  </si>
-  <si>
     <t>robertapplin</t>
   </si>
   <si>
@@ -154,55 +142,13 @@
     <t>No Assigned</t>
   </si>
   <si>
-    <t>Harrietbrown</t>
-  </si>
-  <si>
-    <t>Harriet Brown</t>
-  </si>
-  <si>
-    <t>DanielMurphy22</t>
-  </si>
-  <si>
-    <t>DannyHindson</t>
-  </si>
-  <si>
     <t>RichardWaiteSTFC</t>
   </si>
   <si>
-    <t>StephenSmith25</t>
-  </si>
-  <si>
-    <t>DavidFair</t>
-  </si>
-  <si>
-    <t>David Fair</t>
-  </si>
-  <si>
-    <t>Stephen Smith</t>
-  </si>
-  <si>
-    <t>Daniel Murphy</t>
-  </si>
-  <si>
     <t>Richard Waite</t>
   </si>
   <si>
-    <t>Danny Hindson</t>
-  </si>
-  <si>
     <t>Anthony Lim</t>
-  </si>
-  <si>
-    <t>tolu28-coder</t>
-  </si>
-  <si>
-    <t>Toluwalase Agoro</t>
-  </si>
-  <si>
-    <t>joseph-torsney</t>
-  </si>
-  <si>
-    <t>Joseph Torsney</t>
   </si>
   <si>
     <t>Manual Testing Live Data ORNL</t>
@@ -1108,7 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -1131,80 +1077,80 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1283,13 +1229,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>assignees!$A$2:$A$27</xm:f>
+            <xm:f>assignees!$A$2:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>C10:C29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>assignees!$A$2:$A$28</xm:f>
+            <xm:f>assignees!$A$2:$A$19</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C9</xm:sqref>
         </x14:dataValidation>
@@ -1301,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,21 +1261,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <f>COUNTIF(issues!$C:$C,assignees!A2)</f>
@@ -1338,10 +1284,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <f>COUNTIF(issues!$C:$C,assignees!A3)</f>
@@ -1350,22 +1296,22 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <f>COUNTIF(issues!$C:$C,assignees!A4)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <f>COUNTIF(issues!$C:$C,assignees!A5)</f>
@@ -1374,10 +1320,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <f>COUNTIF(issues!$C:$C,assignees!A6)</f>
@@ -1386,22 +1332,22 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <f>COUNTIF(issues!$C:$C,assignees!A7)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C8">
         <f>COUNTIF(issues!$C:$C,assignees!A8)</f>
@@ -1410,10 +1356,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <f>COUNTIF(issues!$C:$C,assignees!A9)</f>
@@ -1422,10 +1368,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <f>COUNTIF(issues!$C:$C,assignees!A10)</f>
@@ -1434,10 +1380,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <f>COUNTIF(issues!$C:$C,assignees!A11)</f>
@@ -1446,10 +1392,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <f>COUNTIF(issues!$C:$C,assignees!A12)</f>
@@ -1458,10 +1404,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <f>COUNTIF(issues!$C:$C,assignees!A13)</f>
@@ -1470,10 +1416,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <f>COUNTIF(issues!$C:$C,assignees!A14)</f>
@@ -1482,10 +1428,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <f>COUNTIF(issues!$C:$C,assignees!A15)</f>
@@ -1494,10 +1440,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16">
         <f>COUNTIF(issues!$C:$C,assignees!A16)</f>
@@ -1506,10 +1452,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17">
         <f>COUNTIF(issues!$C:$C,assignees!A17)</f>
@@ -1518,10 +1464,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C18">
         <f>COUNTIF(issues!$C:$C,assignees!A18)</f>
@@ -1530,121 +1476,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C19">
         <f>COUNTIF(issues!$C:$C,assignees!A19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20">
-        <f>COUNTIF(issues!$C:$C,assignees!A20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21">
-        <f>COUNTIF(issues!$C:$C,assignees!A21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <f>COUNTIF(issues!$C:$C,assignees!A22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23">
-        <f>COUNTIF(issues!$C:$C,assignees!A23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24">
-        <f>COUNTIF(issues!$C:$C,assignees!A24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25">
-        <f>COUNTIF(issues!$C:$C,assignees!A25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26">
-        <f>COUNTIF(issues!$C:$C,assignees!A26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27">
-        <f>COUNTIF(issues!$C:$C,assignees!A27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28">
-        <f>COUNTIF(issues!$C:$C,assignees!A28)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>